<commit_message>
Léger fix page detail
</commit_message>
<xml_diff>
--- a/public/ArchivesSorties.xlsx
+++ b/public/ArchivesSorties.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>Champ de Mars, 5 rue Anatole-France Paris (75000)</t>
+  </si>
+  <si>
+    <t>test archivage</t>
+  </si>
+  <si>
+    <t>2020-02-28 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-03-01 12:10:00</t>
+  </si>
+  <si>
+    <t>2020-03-11 12:10:00</t>
+  </si>
+  <si>
+    <t>Test d'archivage</t>
+  </si>
+  <si>
+    <t>Place de la fontaine Lille (59000)</t>
   </si>
 </sst>
 </file>
@@ -422,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:K1"/>
@@ -498,6 +516,39 @@
       </c>
       <c r="K2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction fitre date pour blocage affichage sorties passée + 1 mois
</commit_message>
<xml_diff>
--- a/public/ArchivesSorties.xlsx
+++ b/public/ArchivesSorties.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -48,51 +48,6 @@
   </si>
   <si>
     <t>Lieu</t>
-  </si>
-  <si>
-    <t>Visite de Paris</t>
-  </si>
-  <si>
-    <t>2020-12-25 12:19:53</t>
-  </si>
-  <si>
-    <t>2021-01-12 12:19:45</t>
-  </si>
-  <si>
-    <t>2021-01-14 15:54:59</t>
-  </si>
-  <si>
-    <t>Voyage à Paris en bus pour visiter la capitale et ses monuments</t>
-  </si>
-  <si>
-    <t>Drakyn</t>
-  </si>
-  <si>
-    <t>Saint Herblain</t>
-  </si>
-  <si>
-    <t>Ori 2 | RoiDHyrule</t>
-  </si>
-  <si>
-    <t>Champ de Mars, 5 rue Anatole-France Paris (75000)</t>
-  </si>
-  <si>
-    <t>test archivage</t>
-  </si>
-  <si>
-    <t>2020-02-28 00:00:00</t>
-  </si>
-  <si>
-    <t>2020-03-01 12:10:00</t>
-  </si>
-  <si>
-    <t>2020-03-11 12:10:00</t>
-  </si>
-  <si>
-    <t>Test d'archivage</t>
-  </si>
-  <si>
-    <t>Place de la fontaine Lille (59000)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +395,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:K1"/>
@@ -481,74 +436,6 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>